<commit_message>
fix(sales): update KPI calculation and add debug mode
</commit_message>
<xml_diff>
--- a/ESTADOS CUENTAS DE CLIENTES.xlsx
+++ b/ESTADOS CUENTAS DE CLIENTES.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julietapaganini/Documents/00 Marketing e IT/Antigravity/Dashboard Ventas y Clientes OCME/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E494C54A-38B5-3441-BD1F-F08A603F37B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C0DF6DA-3360-D349-B2AD-0BC3440CD8D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37460" yWindow="600" windowWidth="37460" windowHeight="10500" tabRatio="906" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="600" windowWidth="32660" windowHeight="20400" tabRatio="906" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAMPO FUERTE" sheetId="13" state="hidden" r:id="rId1"/>
@@ -1168,7 +1168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1184,6 +1184,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1476,7 +1482,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="165">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1858,6 +1864,25 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Millares" xfId="4" builtinId="3"/>
@@ -8211,7 +8236,7 @@
     <row r="2" spans="2:3" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="158">
         <f ca="1">TODAY()</f>
-        <v>46051</v>
+        <v>46055</v>
       </c>
       <c r="C2" s="158"/>
     </row>
@@ -12470,8 +12495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:N49"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12676,20 +12701,20 @@
       <c r="C9" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="166">
         <v>200001303</v>
       </c>
-      <c r="E9" s="64">
+      <c r="E9" s="165">
         <f t="shared" ref="E9:E23" si="0">+B9+30</f>
         <v>45386</v>
       </c>
-      <c r="F9" s="65">
+      <c r="F9" s="167">
         <v>19949798.77</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="168" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="64" t="s">
+      <c r="H9" s="165" t="s">
         <v>35</v>
       </c>
       <c r="I9" s="86" t="s">
@@ -12705,17 +12730,17 @@
       <c r="C10" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="166">
         <v>200001304</v>
       </c>
-      <c r="E10" s="64">
+      <c r="E10" s="165">
         <f t="shared" si="0"/>
         <v>45386</v>
       </c>
-      <c r="F10" s="65">
+      <c r="F10" s="167">
         <v>1802758.43</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="168" t="s">
         <v>42</v>
       </c>
       <c r="H10" s="68" t="s">
@@ -12734,17 +12759,17 @@
       <c r="C11" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="169">
         <v>200001307</v>
       </c>
-      <c r="E11" s="64">
+      <c r="E11" s="170">
         <f t="shared" si="0"/>
         <v>45406</v>
       </c>
       <c r="F11" s="65">
         <v>4772819.53</v>
       </c>
-      <c r="G11" s="66" t="s">
+      <c r="G11" s="171" t="s">
         <v>50</v>
       </c>
       <c r="H11" s="68" t="s">
@@ -12763,17 +12788,17 @@
       <c r="C12" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="169">
         <v>200001308</v>
       </c>
-      <c r="E12" s="64">
+      <c r="E12" s="170">
         <f t="shared" si="0"/>
         <v>45406</v>
       </c>
       <c r="F12" s="65">
         <v>9144737.9499999993</v>
       </c>
-      <c r="G12" s="66" t="s">
+      <c r="G12" s="171" t="s">
         <v>51</v>
       </c>
       <c r="H12" s="68" t="s">
@@ -12792,17 +12817,17 @@
       <c r="C13" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="63">
+      <c r="D13" s="169">
         <v>200000091</v>
       </c>
-      <c r="E13" s="64">
+      <c r="E13" s="170">
         <f t="shared" si="0"/>
         <v>45407</v>
       </c>
       <c r="F13" s="65">
         <v>-4772819.53</v>
       </c>
-      <c r="G13" s="66" t="s">
+      <c r="G13" s="171" t="s">
         <v>59</v>
       </c>
       <c r="H13" s="68" t="s">
@@ -12821,17 +12846,17 @@
       <c r="C14" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="63">
+      <c r="D14" s="169">
         <v>200000092</v>
       </c>
-      <c r="E14" s="64">
+      <c r="E14" s="170">
         <f t="shared" si="0"/>
         <v>45407</v>
       </c>
       <c r="F14" s="65">
         <v>-9144737.9499999993</v>
       </c>
-      <c r="G14" s="66" t="s">
+      <c r="G14" s="171" t="s">
         <v>60</v>
       </c>
       <c r="H14" s="68" t="s">
@@ -12850,17 +12875,17 @@
       <c r="C15" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="63">
+      <c r="D15" s="166">
         <v>200000097</v>
       </c>
-      <c r="E15" s="64">
+      <c r="E15" s="165">
         <f t="shared" si="0"/>
         <v>45408</v>
       </c>
-      <c r="F15" s="65">
+      <c r="F15" s="167">
         <v>-6449959.9699999997</v>
       </c>
-      <c r="G15" s="66" t="s">
+      <c r="G15" s="168" t="s">
         <v>61</v>
       </c>
       <c r="H15" s="68" t="s">
@@ -15058,8 +15083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B1:N22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -15250,7 +15275,7 @@
       <c r="G8" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="165" t="s">
         <v>324</v>
       </c>
       <c r="I8" s="67"/>

</xml_diff>